<commit_message>
Update Sprint 3 materials after second scrum meeting.
</commit_message>
<xml_diff>
--- a/Scrum Files/Sprint 3/Sprint 3 Burn down chart.xlsx
+++ b/Scrum Files/Sprint 3/Sprint 3 Burn down chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0209D-5B79-4150-9BC7-0280ECB5E3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A91395-B95B-4711-AFE3-213B39C3CC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -792,43 +792,31 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>45601</c:v>
+                  <c:v>45615</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45604</c:v>
+                  <c:v>45618</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45609</c:v>
+                  <c:v>45621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45614</c:v>
+                  <c:v>45627</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45615</c:v>
+                  <c:v>45629</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$14</c:f>
+              <c:f>Sheet1!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,43 +861,31 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>45601</c:v>
+                  <c:v>45615</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45604</c:v>
+                  <c:v>45618</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45609</c:v>
+                  <c:v>45621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45614</c:v>
+                  <c:v>45627</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45615</c:v>
+                  <c:v>45629</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$10:$C$14</c:f>
+              <c:f>Sheet1!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.87</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34.119999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>49.286999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>73.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,43 +930,31 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>45601</c:v>
+                  <c:v>45615</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45604</c:v>
+                  <c:v>45618</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45609</c:v>
+                  <c:v>45621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45614</c:v>
+                  <c:v>45627</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45615</c:v>
+                  <c:v>45629</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$10:$D$14</c:f>
+              <c:f>Sheet1!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75.489999999999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>35.659999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.94</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2705,7 +2669,7 @@
   <dimension ref="A9:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2732,73 +2696,40 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>45601</v>
+        <v>45615</v>
       </c>
       <c r="B10">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="C10">
         <v>0</v>
-      </c>
-      <c r="D10">
-        <v>98.2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>45604</v>
+        <v>45618</v>
       </c>
       <c r="B11">
-        <v>70</v>
+        <f>B10-5-4</f>
+        <v>136</v>
       </c>
       <c r="C11">
-        <v>21.87</v>
-      </c>
-      <c r="D11">
-        <v>75.489999999999995</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>45609</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>34.119999999999997</v>
-      </c>
-      <c r="D12">
-        <v>35.659999999999997</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>45614</v>
-      </c>
-      <c r="B13">
-        <v>34</v>
-      </c>
-      <c r="C13">
-        <v>49.286999999999999</v>
-      </c>
-      <c r="D13">
-        <v>5.94</v>
+        <v>45627</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>45615</v>
-      </c>
-      <c r="B14">
-        <f>B10-64</f>
-        <v>34</v>
-      </c>
-      <c r="C14">
-        <v>73.5</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+        <v>45629</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update Sprint 3 materials and burn down chart after 3rd sprint meeting.
</commit_message>
<xml_diff>
--- a/Scrum Files/Sprint 3/Sprint 3 Burn down chart.xlsx
+++ b/Scrum Files/Sprint 3/Sprint 3 Burn down chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A91395-B95B-4711-AFE3-213B39C3CC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1B4930-EBAF-406F-9A2A-B7F114300A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="16440" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11820" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,10 @@
                   <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>176</c:v>
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,6 +354,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>123.78700000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.28700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,12 +817,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!#REF!</c:f>
+              <c:f>Sheet1!$B$10:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -824,7 +839,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1D1A-48F0-A1E2-E247AE25A44F}"/>
+              <c16:uniqueId val="{00000001-D5B7-4A5C-B521-2B0FFCA86C00}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -880,12 +895,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!#REF!</c:f>
+              <c:f>Sheet1!$C$10:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -893,7 +917,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1D1A-48F0-A1E2-E247AE25A44F}"/>
+              <c16:uniqueId val="{00000002-D5B7-4A5C-B521-2B0FFCA86C00}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -949,12 +973,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!#REF!</c:f>
+              <c:f>Sheet1!$D$10:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -962,7 +998,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1D1A-48F0-A1E2-E247AE25A44F}"/>
+              <c16:uniqueId val="{00000003-D5B7-4A5C-B521-2B0FFCA86C00}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2668,19 +2704,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC08104-6C28-4261-A13C-09D20918E634}">
   <dimension ref="A9:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.9140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2694,7 +2730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45615</v>
       </c>
@@ -2704,8 +2740,11 @@
       <c r="C10">
         <v>0</v>
       </c>
+      <c r="D10">
+        <v>145</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45618</v>
       </c>
@@ -2716,23 +2755,47 @@
       <c r="C11">
         <v>6.5</v>
       </c>
+      <c r="D11">
+        <v>113</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45621</v>
       </c>
+      <c r="B12">
+        <v>122</v>
+      </c>
+      <c r="C12">
+        <v>35.5</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45627</v>
       </c>
+      <c r="B13">
+        <v>88</v>
+      </c>
+      <c r="C13">
+        <v>57.5</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45629</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
@@ -2740,7 +2803,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2754,7 +2817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45587</v>
       </c>
@@ -2768,7 +2831,7 @@
         <v>291.2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45595</v>
       </c>
@@ -2783,7 +2846,7 @@
         <v>235.73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45601</v>
       </c>
@@ -2798,7 +2861,7 @@
         <v>194.13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45608</v>
       </c>
@@ -2814,13 +2877,12 @@
         <v>145.6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45615</v>
       </c>
       <c r="B25">
-        <f>B24-34</f>
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="C25">
         <f>C24+38.5</f>
@@ -2830,15 +2892,22 @@
         <v>97.07</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45622</v>
       </c>
+      <c r="B26">
+        <v>94</v>
+      </c>
+      <c r="C26">
+        <f>C25+49.5</f>
+        <v>173.28700000000001</v>
+      </c>
       <c r="D26">
         <v>48.53</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45629</v>
       </c>

</xml_diff>

<commit_message>
Update Sprint 3 Burn Down Chart.
</commit_message>
<xml_diff>
--- a/Scrum Files/Sprint 3/Sprint 3 Burn down chart.xlsx
+++ b/Scrum Files/Sprint 3/Sprint 3 Burn down chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\admission process\TAMU\Fall 2024\CSCE-331\project-3-team-5b\Scrum Files\Sprint 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamda\Downloads\TAMU\Fall 2024\CSCE331\project-3-team-5b\Scrum Files\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1B4930-EBAF-406F-9A2A-B7F114300A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3698C1B5-F8A5-42D5-8375-58C9881069B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11820" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F8BE15DA-A61D-4C34-8B60-9ED829BB68D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,10 +216,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$21:$A$27</c:f>
+              <c:f>Sheet1!$A$21:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>45587</c:v>
                 </c:pt>
@@ -240,16 +240,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45629</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$B$27</c:f>
+              <c:f>Sheet1!$B$21:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>291.2</c:v>
                 </c:pt>
@@ -267,6 +270,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,10 +315,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$21:$A$27</c:f>
+              <c:f>Sheet1!$A$21:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>45587</c:v>
                 </c:pt>
@@ -330,16 +339,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45629</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$C$27</c:f>
+              <c:f>Sheet1!$C$21:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -357,6 +369,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>173.28700000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>187.78700000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>209.28700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,10 +414,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$21:$A$27</c:f>
+              <c:f>Sheet1!$A$21:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>45587</c:v>
                 </c:pt>
@@ -420,35 +438,41 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45629</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$21:$D$27</c:f>
+              <c:f>Sheet1!$D$21:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>291.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>235.73</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>194.13</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145.6</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.07</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.53</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -675,27 +699,13 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
+            <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:sysClr>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -703,16 +713,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Sprint 2 Burn Down Chart</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 3 Burn Down Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -728,27 +736,13 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
+          <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -793,10 +787,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:f>Sheet1!$A$10:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>45615</c:v>
                 </c:pt>
@@ -811,16 +805,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45629</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$14</c:f>
+              <c:f>Sheet1!$B$10:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>145</c:v>
                 </c:pt>
@@ -832,6 +829,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -839,7 +842,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D5B7-4A5C-B521-2B0FFCA86C00}"/>
+              <c16:uniqueId val="{00000000-5F28-44DA-945A-51115034D0BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -871,10 +874,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:f>Sheet1!$A$10:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>45615</c:v>
                 </c:pt>
@@ -889,16 +892,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45629</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$10:$C$14</c:f>
+              <c:f>Sheet1!$C$10:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -910,6 +916,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,7 +929,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D5B7-4A5C-B521-2B0FFCA86C00}"/>
+              <c16:uniqueId val="{00000001-5F28-44DA-945A-51115034D0BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -949,10 +961,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$A$14</c:f>
+              <c:f>Sheet1!$A$10:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>45615</c:v>
                 </c:pt>
@@ -967,29 +979,35 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45629</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$10:$D$14</c:f>
+              <c:f>Sheet1!$D$10:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>113</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -998,7 +1016,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D5B7-4A5C-B521-2B0FFCA86C00}"/>
+              <c16:uniqueId val="{00000002-5F28-44DA-945A-51115034D0BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1011,11 +1029,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241266368"/>
-        <c:axId val="241266848"/>
+        <c:axId val="79383488"/>
+        <c:axId val="79382048"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="241266368"/>
+        <c:axId val="79383488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,14 +1076,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241266848"/>
+        <c:crossAx val="79382048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="241266848"/>
+        <c:axId val="79382048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241266368"/>
+        <c:crossAx val="79383488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2349,22 +2367,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>500062</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>636270</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>477837</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BEA8509-1A45-A7D0-79DD-2934FAB09F5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2503BABF-F6E1-06A8-2FF2-41D89F6E4361}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2702,18 +2720,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC08104-6C28-4261-A13C-09D20918E634}">
-  <dimension ref="A9:D27"/>
+  <dimension ref="A9:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2756,7 +2774,7 @@
         <v>6.5</v>
       </c>
       <c r="D11">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2770,7 +2788,7 @@
         <v>35.5</v>
       </c>
       <c r="D12">
-        <v>82</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2784,15 +2802,41 @@
         <v>57.5</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45629</v>
       </c>
+      <c r="B14">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>64</v>
+      </c>
       <c r="D14">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45637</v>
+      </c>
+      <c r="B15">
         <v>0</v>
+      </c>
+      <c r="C15">
+        <v>85.5</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <f>49.5-64</f>
+        <v>-14.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2843,7 +2887,7 @@
         <v>21.87</v>
       </c>
       <c r="D22">
-        <v>235.73</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2858,7 +2902,7 @@
         <v>50.286999999999999</v>
       </c>
       <c r="D23">
-        <v>194.13</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2874,7 +2918,7 @@
         <v>85.287000000000006</v>
       </c>
       <c r="D24">
-        <v>145.6</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2889,7 +2933,7 @@
         <v>123.78700000000001</v>
       </c>
       <c r="D25">
-        <v>97.07</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2904,14 +2948,36 @@
         <v>173.28700000000001</v>
       </c>
       <c r="D26">
-        <v>48.53</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45629</v>
       </c>
+      <c r="B27">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <f>C26+14.5</f>
+        <v>187.78700000000001</v>
+      </c>
       <c r="D27">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>45637</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>C25+C15</f>
+        <v>209.28700000000001</v>
+      </c>
+      <c r="D28">
         <v>0</v>
       </c>
     </row>

</xml_diff>